<commit_message>
Adding DOE LPO to the unified data set.
</commit_message>
<xml_diff>
--- a/Output/OSC/EXIM/EXIM_Assistance.xlsx
+++ b/Output/OSC/EXIM/EXIM_Assistance.xlsx
@@ -107,8 +107,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="167" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="168" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="172" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="173" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -147,8 +147,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>